<commit_message>
new parameters from ga concluded
</commit_message>
<xml_diff>
--- a/tests/global_metrics.xlsx
+++ b/tests/global_metrics.xlsx
@@ -510,13 +510,13 @@
         <v>0.0891</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0842</v>
+        <v>0.0693</v>
       </c>
       <c r="E2" t="n">
         <v>0.099</v>
       </c>
       <c r="F2" t="n">
-        <v>0.099</v>
+        <v>0.1089</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -537,10 +537,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0791</v>
+        <v>0.0808</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0316</v>
+        <v>0.0439</v>
       </c>
       <c r="E3" t="n">
         <v>0.0984</v>
@@ -567,16 +567,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0467</v>
+        <v>0.0533</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0267</v>
+        <v>0.0067</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0333</v>
+        <v>0.08</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.073</v>
+        <v>0.0506</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0281</v>
+        <v>0.0169</v>
       </c>
       <c r="E5" t="n">
         <v>0.08989999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0225</v>
+        <v>0.0337</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -631,13 +631,13 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>0.071975</v>
+        <v>0.06845</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000245976875</v>
+        <v>0.0002817725</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01568364992595793</v>
+        <v>0.01678608054311667</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -690,13 +690,13 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
-        <v>0.02843333333333334</v>
+        <v>0.0228</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0007899955555555555</v>
+        <v>0.00065686</v>
       </c>
       <c r="L8" t="n">
-        <v>0.02810685958188064</v>
+        <v>0.02562928013035091</v>
       </c>
     </row>
     <row r="9">
@@ -718,13 +718,13 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>0.03224999999999999</v>
+        <v>0.04355000000000001</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0011122425</v>
+        <v>0.001585495833333333</v>
       </c>
       <c r="L9" t="n">
-        <v>0.03335029984872699</v>
+        <v>0.03981828516314249</v>
       </c>
     </row>
     <row r="10">
@@ -739,16 +739,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0743</v>
+        <v>0.0446</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0693</v>
+        <v>0.0396</v>
       </c>
       <c r="E10" t="n">
         <v>0.099</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0891</v>
+        <v>0.1089</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -769,16 +769,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.09669999999999999</v>
+        <v>0.0861</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0316</v>
+        <v>0.0281</v>
       </c>
       <c r="E11" t="n">
         <v>0.0984</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0439</v>
+        <v>0.0457</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -799,16 +799,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.12</v>
+        <v>0.1067</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0467</v>
+        <v>0.0267</v>
       </c>
       <c r="E12" t="n">
         <v>0.1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
@@ -829,16 +829,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.1236</v>
+        <v>0.1292</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0393</v>
+        <v>0.0281</v>
       </c>
       <c r="E13" t="n">
         <v>0.08989999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0225</v>
+        <v>0.0506</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -863,13 +863,13 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>0.10365</v>
+        <v>0.09165000000000001</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0003937624999999999</v>
+        <v>0.0009702525000000002</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01984344980087888</v>
+        <v>0.03114887638422934</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -922,13 +922,13 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
-        <v>0.03115</v>
+        <v>0.02041666666666667</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0006174158333333334</v>
+        <v>0.0002265380555555556</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0248478536967146</v>
+        <v>0.0150511812013395</v>
       </c>
     </row>
     <row r="17">
@@ -950,13 +950,13 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
-        <v>0.03258333333333333</v>
+        <v>0.0442</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0009337047222222222</v>
+        <v>0.001397703333333333</v>
       </c>
       <c r="L17" t="n">
-        <v>0.03055658230598151</v>
+        <v>0.03738587077136673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tryng to get men values
</commit_message>
<xml_diff>
--- a/tests/global_metrics.xlsx
+++ b/tests/global_metrics.xlsx
@@ -507,16 +507,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0891</v>
+        <v>0.0693</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0693</v>
+        <v>0.0594</v>
       </c>
       <c r="E2" t="n">
         <v>0.099</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1089</v>
+        <v>0.099</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -537,16 +537,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0808</v>
+        <v>0.08790000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0439</v>
+        <v>0.0562</v>
       </c>
       <c r="E3" t="n">
         <v>0.0984</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0387</v>
+        <v>0.0527</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -567,16 +567,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0533</v>
+        <v>0.0333</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0067</v>
+        <v>0.0133</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.08</v>
+        <v>0.0533</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0506</v>
+        <v>0.0618</v>
       </c>
       <c r="D5" t="n">
         <v>0.0169</v>
@@ -606,7 +606,7 @@
         <v>0.08989999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0337</v>
+        <v>0.0281</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -631,13 +631,13 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>0.06845</v>
+        <v>0.06307500000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0002817725</v>
+        <v>0.000385801875</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01678608054311667</v>
+        <v>0.01964183990872546</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -690,13 +690,13 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
-        <v>0.0228</v>
+        <v>0.0243</v>
       </c>
       <c r="K8" t="n">
-        <v>0.00065686</v>
+        <v>0.00060106</v>
       </c>
       <c r="L8" t="n">
-        <v>0.02562928013035091</v>
+        <v>0.02451652503924649</v>
       </c>
     </row>
     <row r="9">
@@ -718,13 +718,13 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>0.04355000000000001</v>
+        <v>0.03885</v>
       </c>
       <c r="K9" t="n">
-        <v>0.001585495833333333</v>
+        <v>0.0011921425</v>
       </c>
       <c r="L9" t="n">
-        <v>0.03981828516314249</v>
+        <v>0.0345274166424307</v>
       </c>
     </row>
     <row r="10">
@@ -739,16 +739,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0446</v>
+        <v>0.0743</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0396</v>
+        <v>0.0693</v>
       </c>
       <c r="E10" t="n">
         <v>0.099</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1089</v>
+        <v>0.0891</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -769,16 +769,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0861</v>
+        <v>0.0914</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0281</v>
+        <v>0.0369</v>
       </c>
       <c r="E11" t="n">
         <v>0.0984</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0457</v>
+        <v>0.0404</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -799,16 +799,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1067</v>
+        <v>0.08</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0267</v>
+        <v>0.0533</v>
       </c>
       <c r="E12" t="n">
         <v>0.1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
@@ -829,16 +829,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.1292</v>
+        <v>0.1236</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0281</v>
+        <v>0.0506</v>
       </c>
       <c r="E13" t="n">
         <v>0.08989999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0506</v>
+        <v>0.0337</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -863,13 +863,13 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>0.09165000000000001</v>
+        <v>0.092325</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0009702525000000002</v>
+        <v>0.000363946875</v>
       </c>
       <c r="I14" t="n">
-        <v>0.03114887638422934</v>
+        <v>0.01907739172423736</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -922,13 +922,13 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
-        <v>0.02041666666666667</v>
+        <v>0.03501666666666667</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0002265380555555556</v>
+        <v>0.0007013913888888889</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0150511812013395</v>
+        <v>0.02648379483550061</v>
       </c>
     </row>
     <row r="17">
@@ -950,13 +950,13 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
-        <v>0.0442</v>
+        <v>0.04053333333333334</v>
       </c>
       <c r="K17" t="n">
-        <v>0.001397703333333333</v>
+        <v>0.001208158888888889</v>
       </c>
       <c r="L17" t="n">
-        <v>0.03738587077136673</v>
+        <v>0.03475858007584443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make test with config 03
</commit_message>
<xml_diff>
--- a/tests/global_metrics.xlsx
+++ b/tests/global_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,50 +446,35 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>original error rate PC_LabelCorrection</t>
+          <t>Erro</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>error rate after correction PC_LabelCorrection</t>
+          <t>before_fix_mean</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>original error rate CL</t>
+          <t>before_fix_variance</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>error rate after correction CL</t>
+          <t>before_fix_std</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>before_fix_mean</t>
+          <t>after_fix_mean</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>before_fix_variance</t>
+          <t>after_fix_variance</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>before_fix_std</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>after_fix_mean</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>after_fix_variance</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>after_fix_std</t>
         </is>
@@ -506,24 +491,17 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0.0693</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0594</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.099</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.099</v>
-      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -536,24 +514,17 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>0.08790000000000001</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0562</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.0984</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.0527</v>
-      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -566,24 +537,17 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0.0333</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0133</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.0533</v>
-      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -596,24 +560,17 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.0618</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0169</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.08989999999999999</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.0281</v>
-      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -627,21 +584,18 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>0.06307500000000001</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.000385801875</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.01964183990872546</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -655,21 +609,18 @@
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>0.09682499999999999</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.631187500000003e-05</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.004038796231552173</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -686,17 +637,14 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
-        <v>0.0243</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.00060106</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.02451652503924649</v>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -714,17 +662,14 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
-        <v>0.03885</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.0011921425</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.0345274166424307</v>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -738,24 +683,17 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>0.0743</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0693</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.099</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0891</v>
-      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -768,24 +706,17 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.0914</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0369</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0984</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.0404</v>
-      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -798,24 +729,17 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0533</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.08</v>
-      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -828,24 +752,17 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>0.1236</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.0506</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.08989999999999999</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.0337</v>
-      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>can't convert type 'dict' to numerator/denominator</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -859,21 +776,18 @@
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
-        <v>0.092325</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.000363946875</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.01907739172423736</v>
-      </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -887,21 +801,18 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>0.09682499999999999</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1.631187500000003e-05</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.004038796231552173</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -918,17 +829,14 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>0.03501666666666667</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.0007013913888888889</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.02648379483550061</v>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -946,17 +854,14 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
-        <v>0.04053333333333334</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.001208158888888889</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.03475858007584443</v>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test before 100 generations
</commit_message>
<xml_diff>
--- a/tests/global_metrics.xlsx
+++ b/tests/global_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,35 +446,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Erro</t>
+          <t>original error rate PC_LabelCorrection</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>error rate after correction PC_LabelCorrection</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>original error rate CL</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>error rate after correction CL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>before_fix_mean</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>before_fix_variance</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>before_fix_std</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>after_fix_mean</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>after_fix_variance</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>after_fix_std</t>
         </is>
@@ -491,17 +506,24 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>can't convert type 'dict' to numerator/denominator</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0.08169</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.04607</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.09702</v>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -514,17 +536,24 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>can't convert type 'dict' to numerator/denominator</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>0.08225</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.03779</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.04482</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -537,17 +566,24 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>tuple index out of range</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>0.05734</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01866</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.058</v>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -560,17 +596,24 @@
           <t>PC</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>can't convert type 'dict' to numerator/denominator</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>0.07417</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.02248</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.08989999999999999</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03371</v>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -584,18 +627,21 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0.0738625</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.00010117686875</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.01005867132130283</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -609,18 +655,21 @@
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0.09682499999999999</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.631187500000003e-05</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.004038796231552173</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -637,14 +686,17 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0002999847222222222</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.01732006703861801</v>
       </c>
     </row>
     <row r="9">
@@ -662,14 +714,17 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>0.03892499999999999</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.001138523858333333</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.03374201917984952</v>
       </c>
     </row>
     <row r="10">
@@ -683,17 +738,24 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>can't convert type 'dict' to numerator/denominator</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>0.06832000000000001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.05545</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.09801</v>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -706,17 +768,24 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>can't convert type 'dict' to numerator/denominator</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>0.09068999999999999</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0355</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.04569</v>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -729,17 +798,24 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>tuple index out of range</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>0.11133</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.03599</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.06399000000000001</v>
+      </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -752,17 +828,24 @@
           <t>LOF</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>can't convert type 'dict' to numerator/denominator</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0.12304</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.03706</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.08989999999999999</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.03482</v>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -776,18 +859,21 @@
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0.09834499999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0004346382249999999</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.02084797891883048</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -801,18 +887,21 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0.09682499999999999</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.631187500000003e-05</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.004038796231552173</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -829,14 +918,17 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>0.02733333333333333</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0004201682555555556</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.02049800613609908</v>
       </c>
     </row>
     <row r="17">
@@ -854,14 +946,17 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0.04041833333333333</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.001199806447222222</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.03463822234500816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>